<commit_message>
Henry works, but density flow it too intense to be true.
</commit_message>
<xml_diff>
--- a/Projects/Density/cases/Henry/Henry.xlsx
+++ b/Projects/Density/cases/Henry/Henry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/GenericInun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Density/cases/Henry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9EDBA2-7E66-0E4E-BDA1-6893561DE4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51EA1F0-41CB-A44F-9EB2-A0383564BFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11860" yWindow="-26760" windowWidth="30600" windowHeight="19860" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,10 @@
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
     <sheet name="SIM6" sheetId="11" r:id="rId2"/>
     <sheet name="GWF6" sheetId="9" r:id="rId3"/>
-    <sheet name="GWT6" sheetId="10" r:id="rId4"/>
-    <sheet name="PER" sheetId="5" r:id="rId5"/>
-    <sheet name="LAY" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId4"/>
+    <sheet name="GWT6" sheetId="10" r:id="rId5"/>
+    <sheet name="PER" sheetId="5" r:id="rId6"/>
+    <sheet name="LAY" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_rch2">#REF!</definedName>
@@ -205,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="421">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1362,42 +1363,6 @@
     <t>METER</t>
   </si>
   <si>
-    <t>Alluviale deklagen</t>
-  </si>
-  <si>
-    <t>Eolisch deklagen buiten Roerdalslenk</t>
-  </si>
-  <si>
-    <t>Pleisocene afzettingen</t>
-  </si>
-  <si>
-    <t>Runsbroek-Berg Aquifer</t>
-  </si>
-  <si>
-    <t>Tongeren Aquitard</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>A0140</t>
-  </si>
-  <si>
-    <t>A0150</t>
-  </si>
-  <si>
-    <t>A0170</t>
-  </si>
-  <si>
-    <t>A0430</t>
-  </si>
-  <si>
-    <t>A0440</t>
-  </si>
-  <si>
     <t>ICELLTYPE</t>
   </si>
   <si>
@@ -1410,37 +1375,106 @@
     <t>Ss</t>
   </si>
   <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>khaki</t>
-  </si>
-  <si>
-    <t>COMPLEX</t>
-  </si>
-  <si>
-    <t>Split</t>
+    <t>MODERATE</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>chd</t>
+  </si>
+  <si>
+    <t>wel</t>
+  </si>
+  <si>
+    <t>uzf</t>
+  </si>
+  <si>
+    <t>sto</t>
+  </si>
+  <si>
+    <t>sfr</t>
+  </si>
+  <si>
+    <t>riv</t>
+  </si>
+  <si>
+    <t>rcha</t>
+  </si>
+  <si>
+    <t>rch</t>
+  </si>
+  <si>
+    <t>oc</t>
+  </si>
+  <si>
+    <t>npf</t>
+  </si>
+  <si>
+    <t>nam</t>
+  </si>
+  <si>
+    <t>mvr</t>
+  </si>
+  <si>
+    <t>maw</t>
+  </si>
+  <si>
+    <t>lak</t>
+  </si>
+  <si>
+    <t>fic</t>
+  </si>
+  <si>
+    <t>gnc</t>
+  </si>
+  <si>
+    <t>ghb</t>
+  </si>
+  <si>
+    <t>evta</t>
+  </si>
+  <si>
+    <t>evt</t>
+  </si>
+  <si>
+    <t>drn</t>
+  </si>
+  <si>
+    <t>disv</t>
+  </si>
+  <si>
+    <t>disu</t>
+  </si>
+  <si>
+    <t>dis</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>ims</t>
+  </si>
+  <si>
+    <t>qL</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>por</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1562,7 +1596,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1582,9 +1616,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1971,8 +2003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2017,11 +2049,11 @@
         <v>256</v>
       </c>
       <c r="B3" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="12" t="str">
         <f>IF(B3=1,"&lt;====","")</f>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>257</v>
@@ -2032,11 +2064,11 @@
         <v>258</v>
       </c>
       <c r="B4" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="12" t="str">
         <f t="shared" ref="C4:C47" si="0">IF(B4=1,"&lt;====","")</f>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>259</v>
@@ -2107,11 +2139,11 @@
         <v>268</v>
       </c>
       <c r="B9" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;====</v>
+        <v/>
       </c>
       <c r="D9" s="12" t="s">
         <v>269</v>
@@ -2287,11 +2319,11 @@
         <v>292</v>
       </c>
       <c r="B21" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;====</v>
+        <v/>
       </c>
       <c r="D21" s="12" t="s">
         <v>293</v>
@@ -2332,11 +2364,11 @@
         <v>298</v>
       </c>
       <c r="B24" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;====</v>
+        <v/>
       </c>
       <c r="D24" s="12" t="s">
         <v>299</v>
@@ -2377,11 +2409,11 @@
         <v>304</v>
       </c>
       <c r="B27" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>305</v>
@@ -2713,7 +2745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9985BC8C-AF94-474C-A200-72B17F25D172}">
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -3547,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A32" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3673,7 +3705,7 @@
         <v>111</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>383</v>
@@ -4005,8 +4037,8 @@
       <c r="B41" t="s">
         <v>33</v>
       </c>
-      <c r="C41" t="s">
-        <v>22</v>
+      <c r="C41" s="11" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
@@ -4115,8 +4147,8 @@
       <c r="B52" t="s">
         <v>34</v>
       </c>
-      <c r="C52" t="s">
-        <v>22</v>
+      <c r="C52" s="11" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
@@ -4269,8 +4301,8 @@
       <c r="B67" t="s">
         <v>34</v>
       </c>
-      <c r="C67" t="s">
-        <v>22</v>
+      <c r="C67" s="11" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -4456,8 +4488,8 @@
       <c r="B85" t="s">
         <v>34</v>
       </c>
-      <c r="C85" t="s">
-        <v>22</v>
+      <c r="C85" s="11" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
@@ -4632,8 +4664,8 @@
       <c r="B102" t="s">
         <v>33</v>
       </c>
-      <c r="C102" t="s">
-        <v>22</v>
+      <c r="C102" s="11" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
@@ -4819,8 +4851,8 @@
       <c r="B120" t="s">
         <v>34</v>
       </c>
-      <c r="C120" t="s">
-        <v>22</v>
+      <c r="C120" s="11" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -4995,8 +5027,8 @@
       <c r="B137" t="s">
         <v>34</v>
       </c>
-      <c r="C137" t="s">
-        <v>22</v>
+      <c r="C137" s="11" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -5182,8 +5214,8 @@
       <c r="B155" t="s">
         <v>34</v>
       </c>
-      <c r="C155" t="s">
-        <v>22</v>
+      <c r="C155" s="11" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
@@ -5380,8 +5412,8 @@
       <c r="B174" t="s">
         <v>34</v>
       </c>
-      <c r="C174" t="s">
-        <v>22</v>
+      <c r="C174" s="11" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
@@ -5545,8 +5577,8 @@
       <c r="B190" t="s">
         <v>34</v>
       </c>
-      <c r="C190" t="s">
-        <v>22</v>
+      <c r="C190" s="11" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
@@ -5710,8 +5742,8 @@
       <c r="B206" t="s">
         <v>34</v>
       </c>
-      <c r="C206" t="s">
-        <v>22</v>
+      <c r="C206" s="11" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
@@ -5832,10 +5864,10 @@
         <v>46</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="D218" s="11" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.15">
@@ -5966,8 +5998,8 @@
       <c r="B232" t="s">
         <v>34</v>
       </c>
-      <c r="C232" t="s">
-        <v>22</v>
+      <c r="C232" s="11" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.15">
@@ -6263,8 +6295,8 @@
       <c r="B260" t="s">
         <v>34</v>
       </c>
-      <c r="C260" t="s">
-        <v>22</v>
+      <c r="C260" s="11" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.15">
@@ -6527,8 +6559,8 @@
       <c r="B285" t="s">
         <v>34</v>
       </c>
-      <c r="C285" t="s">
-        <v>22</v>
+      <c r="C285" s="11" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.15">
@@ -6659,8 +6691,8 @@
       <c r="B298" t="s">
         <v>34</v>
       </c>
-      <c r="C298" t="s">
-        <v>22</v>
+      <c r="C298" s="11" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.15">
@@ -6769,8 +6801,8 @@
       <c r="B309" t="s">
         <v>34</v>
       </c>
-      <c r="C309" t="s">
-        <v>22</v>
+      <c r="C309" s="11" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.15">
@@ -7022,8 +7054,8 @@
       <c r="B333" t="s">
         <v>34</v>
       </c>
-      <c r="C333" t="s">
-        <v>22</v>
+      <c r="C333" s="11" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.15">
@@ -7121,8 +7153,8 @@
       <c r="B343" t="s">
         <v>34</v>
       </c>
-      <c r="C343" t="s">
-        <v>22</v>
+      <c r="C343" s="11" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.15">
@@ -7286,8 +7318,8 @@
       <c r="B359" t="s">
         <v>34</v>
       </c>
-      <c r="C359" t="s">
-        <v>22</v>
+      <c r="C359" s="11" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.15">
@@ -7462,8 +7494,8 @@
       <c r="B376" t="s">
         <v>34</v>
       </c>
-      <c r="C376" t="s">
-        <v>22</v>
+      <c r="C376" s="11" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.15">
@@ -7627,8 +7659,8 @@
       <c r="B392" t="s">
         <v>34</v>
       </c>
-      <c r="C392" t="s">
-        <v>22</v>
+      <c r="C392" s="11" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.15">
@@ -7902,8 +7934,8 @@
       <c r="B418" t="s">
         <v>34</v>
       </c>
-      <c r="C418" t="s">
-        <v>22</v>
+      <c r="C418" s="11" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.15">
@@ -8035,8 +8067,8 @@
       <c r="B431" t="s">
         <v>34</v>
       </c>
-      <c r="C431" t="s">
-        <v>22</v>
+      <c r="C431" s="11" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.15">
@@ -8332,8 +8364,8 @@
       <c r="B459" t="s">
         <v>34</v>
       </c>
-      <c r="C459" t="s">
-        <v>22</v>
+      <c r="C459" s="11" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.15">
@@ -8508,8 +8540,8 @@
       <c r="B476" t="s">
         <v>34</v>
       </c>
-      <c r="C476" t="s">
-        <v>22</v>
+      <c r="C476" s="11" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.15">
@@ -8530,11 +8562,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8446BBDB-199E-EA4C-8CB6-7B333DCEF8D5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="B1" s="2">
+        <v>6.6000000000000003E-6</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="B3" s="11">
+        <f>180*60</f>
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" s="2">
+        <f>B1/B2*B3</f>
+        <v>0.28512000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06ADD67-459A-3448-A388-0C190A7D0288}">
   <dimension ref="A1:D315"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A47" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8699,7 +8783,7 @@
         <v>111</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>383</v>
@@ -11840,12 +11924,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11858,7 +11942,12 @@
       <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="B1" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>390</v>
+      </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -11888,10 +11977,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="15">
-        <v>45292</v>
+        <v>60</v>
       </c>
       <c r="C3" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D3" s="10">
         <v>12</v>
@@ -11908,10 +11997,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="15">
-        <v>45292</v>
+        <f>B3+C4</f>
+        <v>120</v>
       </c>
       <c r="C4" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D4" s="10">
         <v>12</v>
@@ -11928,10 +12018,11 @@
         <v>2</v>
       </c>
       <c r="B5" s="15">
-        <v>45292</v>
+        <f t="shared" ref="B5:B33" si="0">B4+C5</f>
+        <v>180</v>
       </c>
       <c r="C5" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D5" s="10">
         <v>12</v>
@@ -11948,10 +12039,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>240</v>
       </c>
       <c r="C6" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D6" s="10">
         <v>12</v>
@@ -11968,10 +12060,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="C7" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10">
         <v>12</v>
@@ -11985,13 +12078,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="B8" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="C8" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D8" s="10">
         <v>12</v>
@@ -12005,13 +12099,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="B9" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>420</v>
       </c>
       <c r="C9" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D9" s="10">
         <v>12</v>
@@ -12025,13 +12120,14 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="B10" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>480</v>
       </c>
       <c r="C10" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D10" s="10">
         <v>12</v>
@@ -12045,13 +12141,14 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="B11" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>540</v>
       </c>
       <c r="C11" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D11" s="10">
         <v>12</v>
@@ -12065,13 +12162,14 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>9</v>
+        <v>-1</v>
       </c>
       <c r="B12" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>600</v>
       </c>
       <c r="C12" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D12" s="10">
         <v>12</v>
@@ -12085,13 +12183,14 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="B13" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>660</v>
       </c>
       <c r="C13" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D13" s="10">
         <v>12</v>
@@ -12105,13 +12204,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="B14" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>720</v>
       </c>
       <c r="C14" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D14" s="10">
         <v>12</v>
@@ -12125,13 +12225,14 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="B15" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>780</v>
       </c>
       <c r="C15" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D15" s="10">
         <v>12</v>
@@ -12145,13 +12246,14 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>13</v>
+        <v>-1</v>
       </c>
       <c r="B16" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>840</v>
       </c>
       <c r="C16" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D16" s="10">
         <v>12</v>
@@ -12165,13 +12267,14 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>14</v>
+        <v>-1</v>
       </c>
       <c r="B17" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>900</v>
       </c>
       <c r="C17" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D17" s="10">
         <v>12</v>
@@ -12185,13 +12288,14 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>15</v>
+        <v>-1</v>
       </c>
       <c r="B18" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>960</v>
       </c>
       <c r="C18" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D18" s="10">
         <v>12</v>
@@ -12205,13 +12309,14 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>16</v>
+        <v>-1</v>
       </c>
       <c r="B19" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1020</v>
       </c>
       <c r="C19" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D19" s="10">
         <v>12</v>
@@ -12225,13 +12330,14 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>17</v>
+        <v>-1</v>
       </c>
       <c r="B20" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1080</v>
       </c>
       <c r="C20" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D20" s="10">
         <v>12</v>
@@ -12245,13 +12351,14 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>18</v>
+        <v>-1</v>
       </c>
       <c r="B21" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1140</v>
       </c>
       <c r="C21" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D21" s="10">
         <v>12</v>
@@ -12265,13 +12372,14 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>19</v>
+        <v>-1</v>
       </c>
       <c r="B22" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1200</v>
       </c>
       <c r="C22" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D22" s="10">
         <v>12</v>
@@ -12285,13 +12393,14 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>20</v>
+        <v>-1</v>
       </c>
       <c r="B23" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1260</v>
       </c>
       <c r="C23" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D23" s="10">
         <v>12</v>
@@ -12305,13 +12414,14 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>21</v>
+        <v>-1</v>
       </c>
       <c r="B24" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1320</v>
       </c>
       <c r="C24" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D24" s="10">
         <v>12</v>
@@ -12325,13 +12435,14 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>22</v>
+        <v>-1</v>
       </c>
       <c r="B25" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1380</v>
       </c>
       <c r="C25" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D25" s="10">
         <v>12</v>
@@ -12345,13 +12456,14 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>23</v>
+        <v>-1</v>
       </c>
       <c r="B26" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1440</v>
       </c>
       <c r="C26" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D26" s="10">
         <v>12</v>
@@ -12365,13 +12477,14 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>24</v>
+        <v>-1</v>
       </c>
       <c r="B27" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="C27" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D27" s="10">
         <v>12</v>
@@ -12385,13 +12498,14 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>25</v>
+        <v>-1</v>
       </c>
       <c r="B28" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1560</v>
       </c>
       <c r="C28" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D28" s="10">
         <v>12</v>
@@ -12405,13 +12519,14 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>26</v>
+        <v>-1</v>
       </c>
       <c r="B29" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1620</v>
       </c>
       <c r="C29" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D29" s="10">
         <v>12</v>
@@ -12425,13 +12540,14 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>27</v>
+        <v>-1</v>
       </c>
       <c r="B30" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1680</v>
       </c>
       <c r="C30" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D30" s="10">
         <v>12</v>
@@ -12445,13 +12561,14 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>28</v>
+        <v>-1</v>
       </c>
       <c r="B31" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1740</v>
       </c>
       <c r="C31" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D31" s="10">
         <v>12</v>
@@ -12465,13 +12582,14 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>29</v>
+        <v>-1</v>
       </c>
       <c r="B32" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1800</v>
       </c>
       <c r="C32" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D32" s="10">
         <v>12</v>
@@ -12485,13 +12603,14 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="B33" s="15">
-        <v>45292</v>
+        <f t="shared" si="0"/>
+        <v>1860</v>
       </c>
       <c r="C33" s="10">
-        <v>365</v>
+        <v>60</v>
       </c>
       <c r="D33" s="10">
         <v>12</v>
@@ -12504,11 +12623,3140 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B34" s="15"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
+      <c r="A34">
+        <v>-1</v>
+      </c>
+      <c r="B34" s="15">
+        <f t="shared" ref="B34:B97" si="1">B33+C34</f>
+        <v>1920</v>
+      </c>
+      <c r="C34" s="10">
+        <v>60</v>
+      </c>
+      <c r="D34" s="10">
+        <v>12</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>-1</v>
+      </c>
+      <c r="B35" s="15">
+        <f t="shared" si="1"/>
+        <v>1980</v>
+      </c>
+      <c r="C35" s="10">
+        <v>60</v>
+      </c>
+      <c r="D35" s="10">
+        <v>12</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>-1</v>
+      </c>
+      <c r="B36" s="15">
+        <f t="shared" si="1"/>
+        <v>2040</v>
+      </c>
+      <c r="C36" s="10">
+        <v>60</v>
+      </c>
+      <c r="D36" s="10">
+        <v>12</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>-1</v>
+      </c>
+      <c r="B37" s="15">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+      <c r="C37" s="10">
+        <v>60</v>
+      </c>
+      <c r="D37" s="10">
+        <v>12</v>
+      </c>
+      <c r="E37" s="10">
+        <v>1</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>-1</v>
+      </c>
+      <c r="B38" s="15">
+        <f t="shared" si="1"/>
+        <v>2160</v>
+      </c>
+      <c r="C38" s="10">
+        <v>60</v>
+      </c>
+      <c r="D38" s="10">
+        <v>12</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>-1</v>
+      </c>
+      <c r="B39" s="15">
+        <f t="shared" si="1"/>
+        <v>2220</v>
+      </c>
+      <c r="C39" s="10">
+        <v>60</v>
+      </c>
+      <c r="D39" s="10">
+        <v>12</v>
+      </c>
+      <c r="E39" s="10">
+        <v>1</v>
+      </c>
+      <c r="F39" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>-1</v>
+      </c>
+      <c r="B40" s="15">
+        <f t="shared" si="1"/>
+        <v>2280</v>
+      </c>
+      <c r="C40" s="10">
+        <v>60</v>
+      </c>
+      <c r="D40" s="10">
+        <v>12</v>
+      </c>
+      <c r="E40" s="10">
+        <v>1</v>
+      </c>
+      <c r="F40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>-1</v>
+      </c>
+      <c r="B41" s="15">
+        <f t="shared" si="1"/>
+        <v>2340</v>
+      </c>
+      <c r="C41" s="10">
+        <v>60</v>
+      </c>
+      <c r="D41" s="10">
+        <v>12</v>
+      </c>
+      <c r="E41" s="10">
+        <v>1</v>
+      </c>
+      <c r="F41" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>-1</v>
+      </c>
+      <c r="B42" s="15">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+      <c r="C42" s="10">
+        <v>60</v>
+      </c>
+      <c r="D42" s="10">
+        <v>12</v>
+      </c>
+      <c r="E42" s="10">
+        <v>1</v>
+      </c>
+      <c r="F42" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>-1</v>
+      </c>
+      <c r="B43" s="15">
+        <f t="shared" si="1"/>
+        <v>2460</v>
+      </c>
+      <c r="C43" s="10">
+        <v>60</v>
+      </c>
+      <c r="D43" s="10">
+        <v>12</v>
+      </c>
+      <c r="E43" s="10">
+        <v>1</v>
+      </c>
+      <c r="F43" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>-1</v>
+      </c>
+      <c r="B44" s="15">
+        <f t="shared" si="1"/>
+        <v>2520</v>
+      </c>
+      <c r="C44" s="10">
+        <v>60</v>
+      </c>
+      <c r="D44" s="10">
+        <v>12</v>
+      </c>
+      <c r="E44" s="10">
+        <v>1</v>
+      </c>
+      <c r="F44" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>-1</v>
+      </c>
+      <c r="B45" s="15">
+        <f t="shared" si="1"/>
+        <v>2580</v>
+      </c>
+      <c r="C45" s="10">
+        <v>60</v>
+      </c>
+      <c r="D45" s="10">
+        <v>12</v>
+      </c>
+      <c r="E45" s="10">
+        <v>1</v>
+      </c>
+      <c r="F45" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>-1</v>
+      </c>
+      <c r="B46" s="15">
+        <f t="shared" si="1"/>
+        <v>2640</v>
+      </c>
+      <c r="C46" s="10">
+        <v>60</v>
+      </c>
+      <c r="D46" s="10">
+        <v>12</v>
+      </c>
+      <c r="E46" s="10">
+        <v>1</v>
+      </c>
+      <c r="F46" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>-1</v>
+      </c>
+      <c r="B47" s="15">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+      <c r="C47" s="10">
+        <v>60</v>
+      </c>
+      <c r="D47" s="10">
+        <v>12</v>
+      </c>
+      <c r="E47" s="10">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>-1</v>
+      </c>
+      <c r="B48" s="15">
+        <f t="shared" si="1"/>
+        <v>2760</v>
+      </c>
+      <c r="C48" s="10">
+        <v>60</v>
+      </c>
+      <c r="D48" s="10">
+        <v>12</v>
+      </c>
+      <c r="E48" s="10">
+        <v>1</v>
+      </c>
+      <c r="F48" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>-1</v>
+      </c>
+      <c r="B49" s="15">
+        <f t="shared" si="1"/>
+        <v>2820</v>
+      </c>
+      <c r="C49" s="10">
+        <v>60</v>
+      </c>
+      <c r="D49" s="10">
+        <v>12</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>-1</v>
+      </c>
+      <c r="B50" s="15">
+        <f t="shared" si="1"/>
+        <v>2880</v>
+      </c>
+      <c r="C50" s="10">
+        <v>60</v>
+      </c>
+      <c r="D50" s="10">
+        <v>12</v>
+      </c>
+      <c r="E50" s="10">
+        <v>1</v>
+      </c>
+      <c r="F50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>-1</v>
+      </c>
+      <c r="B51" s="15">
+        <f t="shared" si="1"/>
+        <v>2940</v>
+      </c>
+      <c r="C51" s="10">
+        <v>60</v>
+      </c>
+      <c r="D51" s="10">
+        <v>12</v>
+      </c>
+      <c r="E51" s="10">
+        <v>1</v>
+      </c>
+      <c r="F51" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>-1</v>
+      </c>
+      <c r="B52" s="15">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="C52" s="10">
+        <v>60</v>
+      </c>
+      <c r="D52" s="10">
+        <v>12</v>
+      </c>
+      <c r="E52" s="10">
+        <v>1</v>
+      </c>
+      <c r="F52" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>-1</v>
+      </c>
+      <c r="B53" s="15">
+        <f t="shared" si="1"/>
+        <v>3060</v>
+      </c>
+      <c r="C53" s="10">
+        <v>60</v>
+      </c>
+      <c r="D53" s="10">
+        <v>12</v>
+      </c>
+      <c r="E53" s="10">
+        <v>1</v>
+      </c>
+      <c r="F53" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>-1</v>
+      </c>
+      <c r="B54" s="15">
+        <f t="shared" si="1"/>
+        <v>3120</v>
+      </c>
+      <c r="C54" s="10">
+        <v>60</v>
+      </c>
+      <c r="D54" s="10">
+        <v>12</v>
+      </c>
+      <c r="E54" s="10">
+        <v>1</v>
+      </c>
+      <c r="F54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>-1</v>
+      </c>
+      <c r="B55" s="15">
+        <f t="shared" si="1"/>
+        <v>3180</v>
+      </c>
+      <c r="C55" s="10">
+        <v>60</v>
+      </c>
+      <c r="D55" s="10">
+        <v>12</v>
+      </c>
+      <c r="E55" s="10">
+        <v>1</v>
+      </c>
+      <c r="F55" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>-1</v>
+      </c>
+      <c r="B56" s="15">
+        <f t="shared" si="1"/>
+        <v>3240</v>
+      </c>
+      <c r="C56" s="10">
+        <v>60</v>
+      </c>
+      <c r="D56" s="10">
+        <v>12</v>
+      </c>
+      <c r="E56" s="10">
+        <v>1</v>
+      </c>
+      <c r="F56" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57">
+        <v>-1</v>
+      </c>
+      <c r="B57" s="15">
+        <f t="shared" si="1"/>
+        <v>3300</v>
+      </c>
+      <c r="C57" s="10">
+        <v>60</v>
+      </c>
+      <c r="D57" s="10">
+        <v>12</v>
+      </c>
+      <c r="E57" s="10">
+        <v>1</v>
+      </c>
+      <c r="F57" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58">
+        <v>-1</v>
+      </c>
+      <c r="B58" s="15">
+        <f t="shared" si="1"/>
+        <v>3360</v>
+      </c>
+      <c r="C58" s="10">
+        <v>60</v>
+      </c>
+      <c r="D58" s="10">
+        <v>12</v>
+      </c>
+      <c r="E58" s="10">
+        <v>1</v>
+      </c>
+      <c r="F58" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59">
+        <v>-1</v>
+      </c>
+      <c r="B59" s="15">
+        <f t="shared" si="1"/>
+        <v>3420</v>
+      </c>
+      <c r="C59" s="10">
+        <v>60</v>
+      </c>
+      <c r="D59" s="10">
+        <v>12</v>
+      </c>
+      <c r="E59" s="10">
+        <v>1</v>
+      </c>
+      <c r="F59" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60">
+        <v>-1</v>
+      </c>
+      <c r="B60" s="15">
+        <f t="shared" si="1"/>
+        <v>3480</v>
+      </c>
+      <c r="C60" s="10">
+        <v>60</v>
+      </c>
+      <c r="D60" s="10">
+        <v>12</v>
+      </c>
+      <c r="E60" s="10">
+        <v>1</v>
+      </c>
+      <c r="F60" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61">
+        <v>-1</v>
+      </c>
+      <c r="B61" s="15">
+        <f t="shared" si="1"/>
+        <v>3540</v>
+      </c>
+      <c r="C61" s="10">
+        <v>60</v>
+      </c>
+      <c r="D61" s="10">
+        <v>12</v>
+      </c>
+      <c r="E61" s="10">
+        <v>1</v>
+      </c>
+      <c r="F61" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>-1</v>
+      </c>
+      <c r="B62" s="15">
+        <f t="shared" si="1"/>
+        <v>3600</v>
+      </c>
+      <c r="C62" s="10">
+        <v>60</v>
+      </c>
+      <c r="D62" s="10">
+        <v>12</v>
+      </c>
+      <c r="E62" s="10">
+        <v>1</v>
+      </c>
+      <c r="F62" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>-1</v>
+      </c>
+      <c r="B63" s="15">
+        <f t="shared" si="1"/>
+        <v>3660</v>
+      </c>
+      <c r="C63" s="10">
+        <v>60</v>
+      </c>
+      <c r="D63" s="10">
+        <v>12</v>
+      </c>
+      <c r="E63" s="10">
+        <v>1</v>
+      </c>
+      <c r="F63" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>-1</v>
+      </c>
+      <c r="B64" s="15">
+        <f t="shared" si="1"/>
+        <v>3720</v>
+      </c>
+      <c r="C64" s="10">
+        <v>60</v>
+      </c>
+      <c r="D64" s="10">
+        <v>12</v>
+      </c>
+      <c r="E64" s="10">
+        <v>1</v>
+      </c>
+      <c r="F64" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65">
+        <v>-1</v>
+      </c>
+      <c r="B65" s="15">
+        <f t="shared" si="1"/>
+        <v>3780</v>
+      </c>
+      <c r="C65" s="10">
+        <v>60</v>
+      </c>
+      <c r="D65" s="10">
+        <v>12</v>
+      </c>
+      <c r="E65" s="10">
+        <v>1</v>
+      </c>
+      <c r="F65" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>-1</v>
+      </c>
+      <c r="B66" s="15">
+        <f t="shared" si="1"/>
+        <v>3840</v>
+      </c>
+      <c r="C66" s="10">
+        <v>60</v>
+      </c>
+      <c r="D66" s="10">
+        <v>12</v>
+      </c>
+      <c r="E66" s="10">
+        <v>1</v>
+      </c>
+      <c r="F66" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67">
+        <v>-1</v>
+      </c>
+      <c r="B67" s="15">
+        <f t="shared" si="1"/>
+        <v>3900</v>
+      </c>
+      <c r="C67" s="10">
+        <v>60</v>
+      </c>
+      <c r="D67" s="10">
+        <v>12</v>
+      </c>
+      <c r="E67" s="10">
+        <v>1</v>
+      </c>
+      <c r="F67" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68">
+        <v>-1</v>
+      </c>
+      <c r="B68" s="15">
+        <f t="shared" si="1"/>
+        <v>3960</v>
+      </c>
+      <c r="C68" s="10">
+        <v>60</v>
+      </c>
+      <c r="D68" s="10">
+        <v>12</v>
+      </c>
+      <c r="E68" s="10">
+        <v>1</v>
+      </c>
+      <c r="F68" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A69">
+        <v>-1</v>
+      </c>
+      <c r="B69" s="15">
+        <f t="shared" si="1"/>
+        <v>4020</v>
+      </c>
+      <c r="C69" s="10">
+        <v>60</v>
+      </c>
+      <c r="D69" s="10">
+        <v>12</v>
+      </c>
+      <c r="E69" s="10">
+        <v>1</v>
+      </c>
+      <c r="F69" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A70">
+        <v>-1</v>
+      </c>
+      <c r="B70" s="15">
+        <f t="shared" si="1"/>
+        <v>4080</v>
+      </c>
+      <c r="C70" s="10">
+        <v>60</v>
+      </c>
+      <c r="D70" s="10">
+        <v>12</v>
+      </c>
+      <c r="E70" s="10">
+        <v>1</v>
+      </c>
+      <c r="F70" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A71">
+        <v>-1</v>
+      </c>
+      <c r="B71" s="15">
+        <f t="shared" si="1"/>
+        <v>4140</v>
+      </c>
+      <c r="C71" s="10">
+        <v>60</v>
+      </c>
+      <c r="D71" s="10">
+        <v>12</v>
+      </c>
+      <c r="E71" s="10">
+        <v>1</v>
+      </c>
+      <c r="F71" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A72">
+        <v>-1</v>
+      </c>
+      <c r="B72" s="15">
+        <f t="shared" si="1"/>
+        <v>4200</v>
+      </c>
+      <c r="C72" s="10">
+        <v>60</v>
+      </c>
+      <c r="D72" s="10">
+        <v>12</v>
+      </c>
+      <c r="E72" s="10">
+        <v>1</v>
+      </c>
+      <c r="F72" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A73">
+        <v>-1</v>
+      </c>
+      <c r="B73" s="15">
+        <f t="shared" si="1"/>
+        <v>4260</v>
+      </c>
+      <c r="C73" s="10">
+        <v>60</v>
+      </c>
+      <c r="D73" s="10">
+        <v>12</v>
+      </c>
+      <c r="E73" s="10">
+        <v>1</v>
+      </c>
+      <c r="F73" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A74">
+        <v>-1</v>
+      </c>
+      <c r="B74" s="15">
+        <f t="shared" si="1"/>
+        <v>4320</v>
+      </c>
+      <c r="C74" s="10">
+        <v>60</v>
+      </c>
+      <c r="D74" s="10">
+        <v>12</v>
+      </c>
+      <c r="E74" s="10">
+        <v>1</v>
+      </c>
+      <c r="F74" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A75">
+        <v>-1</v>
+      </c>
+      <c r="B75" s="15">
+        <f t="shared" si="1"/>
+        <v>4380</v>
+      </c>
+      <c r="C75" s="10">
+        <v>60</v>
+      </c>
+      <c r="D75" s="10">
+        <v>12</v>
+      </c>
+      <c r="E75" s="10">
+        <v>1</v>
+      </c>
+      <c r="F75" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A76">
+        <v>-1</v>
+      </c>
+      <c r="B76" s="15">
+        <f t="shared" si="1"/>
+        <v>4440</v>
+      </c>
+      <c r="C76" s="10">
+        <v>60</v>
+      </c>
+      <c r="D76" s="10">
+        <v>12</v>
+      </c>
+      <c r="E76" s="10">
+        <v>1</v>
+      </c>
+      <c r="F76" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A77">
+        <v>-1</v>
+      </c>
+      <c r="B77" s="15">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="C77" s="10">
+        <v>60</v>
+      </c>
+      <c r="D77" s="10">
+        <v>12</v>
+      </c>
+      <c r="E77" s="10">
+        <v>1</v>
+      </c>
+      <c r="F77" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A78">
+        <v>-1</v>
+      </c>
+      <c r="B78" s="15">
+        <f t="shared" si="1"/>
+        <v>4560</v>
+      </c>
+      <c r="C78" s="10">
+        <v>60</v>
+      </c>
+      <c r="D78" s="10">
+        <v>12</v>
+      </c>
+      <c r="E78" s="10">
+        <v>1</v>
+      </c>
+      <c r="F78" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A79">
+        <v>-1</v>
+      </c>
+      <c r="B79" s="15">
+        <f t="shared" si="1"/>
+        <v>4620</v>
+      </c>
+      <c r="C79" s="10">
+        <v>60</v>
+      </c>
+      <c r="D79" s="10">
+        <v>12</v>
+      </c>
+      <c r="E79" s="10">
+        <v>1</v>
+      </c>
+      <c r="F79" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A80">
+        <v>-1</v>
+      </c>
+      <c r="B80" s="15">
+        <f t="shared" si="1"/>
+        <v>4680</v>
+      </c>
+      <c r="C80" s="10">
+        <v>60</v>
+      </c>
+      <c r="D80" s="10">
+        <v>12</v>
+      </c>
+      <c r="E80" s="10">
+        <v>1</v>
+      </c>
+      <c r="F80" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A81">
+        <v>-1</v>
+      </c>
+      <c r="B81" s="15">
+        <f t="shared" si="1"/>
+        <v>4740</v>
+      </c>
+      <c r="C81" s="10">
+        <v>60</v>
+      </c>
+      <c r="D81" s="10">
+        <v>12</v>
+      </c>
+      <c r="E81" s="10">
+        <v>1</v>
+      </c>
+      <c r="F81" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A82">
+        <v>-1</v>
+      </c>
+      <c r="B82" s="15">
+        <f t="shared" si="1"/>
+        <v>4800</v>
+      </c>
+      <c r="C82" s="10">
+        <v>60</v>
+      </c>
+      <c r="D82" s="10">
+        <v>12</v>
+      </c>
+      <c r="E82" s="10">
+        <v>1</v>
+      </c>
+      <c r="F82" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A83">
+        <v>-1</v>
+      </c>
+      <c r="B83" s="15">
+        <f t="shared" si="1"/>
+        <v>4860</v>
+      </c>
+      <c r="C83" s="10">
+        <v>60</v>
+      </c>
+      <c r="D83" s="10">
+        <v>12</v>
+      </c>
+      <c r="E83" s="10">
+        <v>1</v>
+      </c>
+      <c r="F83" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A84">
+        <v>-1</v>
+      </c>
+      <c r="B84" s="15">
+        <f t="shared" si="1"/>
+        <v>4920</v>
+      </c>
+      <c r="C84" s="10">
+        <v>60</v>
+      </c>
+      <c r="D84" s="10">
+        <v>12</v>
+      </c>
+      <c r="E84" s="10">
+        <v>1</v>
+      </c>
+      <c r="F84" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A85">
+        <v>-1</v>
+      </c>
+      <c r="B85" s="15">
+        <f t="shared" si="1"/>
+        <v>4980</v>
+      </c>
+      <c r="C85" s="10">
+        <v>60</v>
+      </c>
+      <c r="D85" s="10">
+        <v>12</v>
+      </c>
+      <c r="E85" s="10">
+        <v>1</v>
+      </c>
+      <c r="F85" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A86">
+        <v>-1</v>
+      </c>
+      <c r="B86" s="15">
+        <f t="shared" si="1"/>
+        <v>5040</v>
+      </c>
+      <c r="C86" s="10">
+        <v>60</v>
+      </c>
+      <c r="D86" s="10">
+        <v>12</v>
+      </c>
+      <c r="E86" s="10">
+        <v>1</v>
+      </c>
+      <c r="F86" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A87">
+        <v>-1</v>
+      </c>
+      <c r="B87" s="15">
+        <f t="shared" si="1"/>
+        <v>5100</v>
+      </c>
+      <c r="C87" s="10">
+        <v>60</v>
+      </c>
+      <c r="D87" s="10">
+        <v>12</v>
+      </c>
+      <c r="E87" s="10">
+        <v>1</v>
+      </c>
+      <c r="F87" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A88">
+        <v>-1</v>
+      </c>
+      <c r="B88" s="15">
+        <f t="shared" si="1"/>
+        <v>5160</v>
+      </c>
+      <c r="C88" s="10">
+        <v>60</v>
+      </c>
+      <c r="D88" s="10">
+        <v>12</v>
+      </c>
+      <c r="E88" s="10">
+        <v>1</v>
+      </c>
+      <c r="F88" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89">
+        <v>-1</v>
+      </c>
+      <c r="B89" s="15">
+        <f t="shared" si="1"/>
+        <v>5220</v>
+      </c>
+      <c r="C89" s="10">
+        <v>60</v>
+      </c>
+      <c r="D89" s="10">
+        <v>12</v>
+      </c>
+      <c r="E89" s="10">
+        <v>1</v>
+      </c>
+      <c r="F89" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A90">
+        <v>-1</v>
+      </c>
+      <c r="B90" s="15">
+        <f t="shared" si="1"/>
+        <v>5280</v>
+      </c>
+      <c r="C90" s="10">
+        <v>60</v>
+      </c>
+      <c r="D90" s="10">
+        <v>12</v>
+      </c>
+      <c r="E90" s="10">
+        <v>1</v>
+      </c>
+      <c r="F90" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A91">
+        <v>-1</v>
+      </c>
+      <c r="B91" s="15">
+        <f t="shared" si="1"/>
+        <v>5340</v>
+      </c>
+      <c r="C91" s="10">
+        <v>60</v>
+      </c>
+      <c r="D91" s="10">
+        <v>12</v>
+      </c>
+      <c r="E91" s="10">
+        <v>1</v>
+      </c>
+      <c r="F91" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A92">
+        <v>-1</v>
+      </c>
+      <c r="B92" s="15">
+        <f t="shared" si="1"/>
+        <v>5400</v>
+      </c>
+      <c r="C92" s="10">
+        <v>60</v>
+      </c>
+      <c r="D92" s="10">
+        <v>12</v>
+      </c>
+      <c r="E92" s="10">
+        <v>1</v>
+      </c>
+      <c r="F92" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A93">
+        <v>-1</v>
+      </c>
+      <c r="B93" s="15">
+        <f t="shared" si="1"/>
+        <v>5460</v>
+      </c>
+      <c r="C93" s="10">
+        <v>60</v>
+      </c>
+      <c r="D93" s="10">
+        <v>12</v>
+      </c>
+      <c r="E93" s="10">
+        <v>1</v>
+      </c>
+      <c r="F93" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A94">
+        <v>-1</v>
+      </c>
+      <c r="B94" s="15">
+        <f t="shared" si="1"/>
+        <v>5520</v>
+      </c>
+      <c r="C94" s="10">
+        <v>60</v>
+      </c>
+      <c r="D94" s="10">
+        <v>12</v>
+      </c>
+      <c r="E94" s="10">
+        <v>1</v>
+      </c>
+      <c r="F94" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A95">
+        <v>-1</v>
+      </c>
+      <c r="B95" s="15">
+        <f t="shared" si="1"/>
+        <v>5580</v>
+      </c>
+      <c r="C95" s="10">
+        <v>60</v>
+      </c>
+      <c r="D95" s="10">
+        <v>12</v>
+      </c>
+      <c r="E95" s="10">
+        <v>1</v>
+      </c>
+      <c r="F95" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A96">
+        <v>-1</v>
+      </c>
+      <c r="B96" s="15">
+        <f t="shared" si="1"/>
+        <v>5640</v>
+      </c>
+      <c r="C96" s="10">
+        <v>60</v>
+      </c>
+      <c r="D96" s="10">
+        <v>12</v>
+      </c>
+      <c r="E96" s="10">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A97">
+        <v>-1</v>
+      </c>
+      <c r="B97" s="15">
+        <f t="shared" si="1"/>
+        <v>5700</v>
+      </c>
+      <c r="C97" s="10">
+        <v>60</v>
+      </c>
+      <c r="D97" s="10">
+        <v>12</v>
+      </c>
+      <c r="E97" s="10">
+        <v>1</v>
+      </c>
+      <c r="F97" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A98">
+        <v>-1</v>
+      </c>
+      <c r="B98" s="15">
+        <f t="shared" ref="B98:B161" si="2">B97+C98</f>
+        <v>5760</v>
+      </c>
+      <c r="C98" s="10">
+        <v>60</v>
+      </c>
+      <c r="D98" s="10">
+        <v>12</v>
+      </c>
+      <c r="E98" s="10">
+        <v>1</v>
+      </c>
+      <c r="F98" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A99">
+        <v>-1</v>
+      </c>
+      <c r="B99" s="15">
+        <f t="shared" si="2"/>
+        <v>5820</v>
+      </c>
+      <c r="C99" s="10">
+        <v>60</v>
+      </c>
+      <c r="D99" s="10">
+        <v>12</v>
+      </c>
+      <c r="E99" s="10">
+        <v>1</v>
+      </c>
+      <c r="F99" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A100">
+        <v>-1</v>
+      </c>
+      <c r="B100" s="15">
+        <f t="shared" si="2"/>
+        <v>5880</v>
+      </c>
+      <c r="C100" s="10">
+        <v>60</v>
+      </c>
+      <c r="D100" s="10">
+        <v>12</v>
+      </c>
+      <c r="E100" s="10">
+        <v>1</v>
+      </c>
+      <c r="F100" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A101">
+        <v>-1</v>
+      </c>
+      <c r="B101" s="15">
+        <f t="shared" si="2"/>
+        <v>5940</v>
+      </c>
+      <c r="C101" s="10">
+        <v>60</v>
+      </c>
+      <c r="D101" s="10">
+        <v>12</v>
+      </c>
+      <c r="E101" s="10">
+        <v>1</v>
+      </c>
+      <c r="F101" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A102">
+        <v>-1</v>
+      </c>
+      <c r="B102" s="15">
+        <f t="shared" si="2"/>
+        <v>6000</v>
+      </c>
+      <c r="C102" s="10">
+        <v>60</v>
+      </c>
+      <c r="D102" s="10">
+        <v>12</v>
+      </c>
+      <c r="E102" s="10">
+        <v>1</v>
+      </c>
+      <c r="F102" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A103">
+        <v>-1</v>
+      </c>
+      <c r="B103" s="15">
+        <f t="shared" si="2"/>
+        <v>6060</v>
+      </c>
+      <c r="C103" s="10">
+        <v>60</v>
+      </c>
+      <c r="D103" s="10">
+        <v>12</v>
+      </c>
+      <c r="E103" s="10">
+        <v>1</v>
+      </c>
+      <c r="F103" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A104">
+        <v>-1</v>
+      </c>
+      <c r="B104" s="15">
+        <f t="shared" si="2"/>
+        <v>6120</v>
+      </c>
+      <c r="C104" s="10">
+        <v>60</v>
+      </c>
+      <c r="D104" s="10">
+        <v>12</v>
+      </c>
+      <c r="E104" s="10">
+        <v>1</v>
+      </c>
+      <c r="F104" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A105">
+        <v>-1</v>
+      </c>
+      <c r="B105" s="15">
+        <f t="shared" si="2"/>
+        <v>6180</v>
+      </c>
+      <c r="C105" s="10">
+        <v>60</v>
+      </c>
+      <c r="D105" s="10">
+        <v>12</v>
+      </c>
+      <c r="E105" s="10">
+        <v>1</v>
+      </c>
+      <c r="F105" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A106">
+        <v>-1</v>
+      </c>
+      <c r="B106" s="15">
+        <f t="shared" si="2"/>
+        <v>6240</v>
+      </c>
+      <c r="C106" s="10">
+        <v>60</v>
+      </c>
+      <c r="D106" s="10">
+        <v>12</v>
+      </c>
+      <c r="E106" s="10">
+        <v>1</v>
+      </c>
+      <c r="F106" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A107">
+        <v>-1</v>
+      </c>
+      <c r="B107" s="15">
+        <f t="shared" si="2"/>
+        <v>6300</v>
+      </c>
+      <c r="C107" s="10">
+        <v>60</v>
+      </c>
+      <c r="D107" s="10">
+        <v>12</v>
+      </c>
+      <c r="E107" s="10">
+        <v>1</v>
+      </c>
+      <c r="F107" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A108">
+        <v>-1</v>
+      </c>
+      <c r="B108" s="15">
+        <f t="shared" si="2"/>
+        <v>6360</v>
+      </c>
+      <c r="C108" s="10">
+        <v>60</v>
+      </c>
+      <c r="D108" s="10">
+        <v>12</v>
+      </c>
+      <c r="E108" s="10">
+        <v>1</v>
+      </c>
+      <c r="F108" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A109">
+        <v>-1</v>
+      </c>
+      <c r="B109" s="15">
+        <f t="shared" si="2"/>
+        <v>6420</v>
+      </c>
+      <c r="C109" s="10">
+        <v>60</v>
+      </c>
+      <c r="D109" s="10">
+        <v>12</v>
+      </c>
+      <c r="E109" s="10">
+        <v>1</v>
+      </c>
+      <c r="F109" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A110">
+        <v>-1</v>
+      </c>
+      <c r="B110" s="15">
+        <f t="shared" si="2"/>
+        <v>6480</v>
+      </c>
+      <c r="C110" s="10">
+        <v>60</v>
+      </c>
+      <c r="D110" s="10">
+        <v>12</v>
+      </c>
+      <c r="E110" s="10">
+        <v>1</v>
+      </c>
+      <c r="F110" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A111">
+        <v>-1</v>
+      </c>
+      <c r="B111" s="15">
+        <f t="shared" si="2"/>
+        <v>6540</v>
+      </c>
+      <c r="C111" s="10">
+        <v>60</v>
+      </c>
+      <c r="D111" s="10">
+        <v>12</v>
+      </c>
+      <c r="E111" s="10">
+        <v>1</v>
+      </c>
+      <c r="F111" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A112">
+        <v>-1</v>
+      </c>
+      <c r="B112" s="15">
+        <f t="shared" si="2"/>
+        <v>6600</v>
+      </c>
+      <c r="C112" s="10">
+        <v>60</v>
+      </c>
+      <c r="D112" s="10">
+        <v>12</v>
+      </c>
+      <c r="E112" s="10">
+        <v>1</v>
+      </c>
+      <c r="F112" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A113">
+        <v>-1</v>
+      </c>
+      <c r="B113" s="15">
+        <f t="shared" si="2"/>
+        <v>6660</v>
+      </c>
+      <c r="C113" s="10">
+        <v>60</v>
+      </c>
+      <c r="D113" s="10">
+        <v>12</v>
+      </c>
+      <c r="E113" s="10">
+        <v>1</v>
+      </c>
+      <c r="F113" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A114">
+        <v>-1</v>
+      </c>
+      <c r="B114" s="15">
+        <f t="shared" si="2"/>
+        <v>6720</v>
+      </c>
+      <c r="C114" s="10">
+        <v>60</v>
+      </c>
+      <c r="D114" s="10">
+        <v>12</v>
+      </c>
+      <c r="E114" s="10">
+        <v>1</v>
+      </c>
+      <c r="F114" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A115">
+        <v>-1</v>
+      </c>
+      <c r="B115" s="15">
+        <f t="shared" si="2"/>
+        <v>6780</v>
+      </c>
+      <c r="C115" s="10">
+        <v>60</v>
+      </c>
+      <c r="D115" s="10">
+        <v>12</v>
+      </c>
+      <c r="E115" s="10">
+        <v>1</v>
+      </c>
+      <c r="F115" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A116">
+        <v>-1</v>
+      </c>
+      <c r="B116" s="15">
+        <f t="shared" si="2"/>
+        <v>6840</v>
+      </c>
+      <c r="C116" s="10">
+        <v>60</v>
+      </c>
+      <c r="D116" s="10">
+        <v>12</v>
+      </c>
+      <c r="E116" s="10">
+        <v>1</v>
+      </c>
+      <c r="F116" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A117">
+        <v>-1</v>
+      </c>
+      <c r="B117" s="15">
+        <f t="shared" si="2"/>
+        <v>6900</v>
+      </c>
+      <c r="C117" s="10">
+        <v>60</v>
+      </c>
+      <c r="D117" s="10">
+        <v>12</v>
+      </c>
+      <c r="E117" s="10">
+        <v>1</v>
+      </c>
+      <c r="F117" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A118">
+        <v>-1</v>
+      </c>
+      <c r="B118" s="15">
+        <f t="shared" si="2"/>
+        <v>6960</v>
+      </c>
+      <c r="C118" s="10">
+        <v>60</v>
+      </c>
+      <c r="D118" s="10">
+        <v>12</v>
+      </c>
+      <c r="E118" s="10">
+        <v>1</v>
+      </c>
+      <c r="F118" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A119">
+        <v>-1</v>
+      </c>
+      <c r="B119" s="15">
+        <f t="shared" si="2"/>
+        <v>7020</v>
+      </c>
+      <c r="C119" s="10">
+        <v>60</v>
+      </c>
+      <c r="D119" s="10">
+        <v>12</v>
+      </c>
+      <c r="E119" s="10">
+        <v>1</v>
+      </c>
+      <c r="F119" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120">
+        <v>-1</v>
+      </c>
+      <c r="B120" s="15">
+        <f t="shared" si="2"/>
+        <v>7080</v>
+      </c>
+      <c r="C120" s="10">
+        <v>60</v>
+      </c>
+      <c r="D120" s="10">
+        <v>12</v>
+      </c>
+      <c r="E120" s="10">
+        <v>1</v>
+      </c>
+      <c r="F120" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121">
+        <v>-1</v>
+      </c>
+      <c r="B121" s="15">
+        <f t="shared" si="2"/>
+        <v>7140</v>
+      </c>
+      <c r="C121" s="10">
+        <v>60</v>
+      </c>
+      <c r="D121" s="10">
+        <v>12</v>
+      </c>
+      <c r="E121" s="10">
+        <v>1</v>
+      </c>
+      <c r="F121" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122">
+        <v>-1</v>
+      </c>
+      <c r="B122" s="15">
+        <f t="shared" si="2"/>
+        <v>7200</v>
+      </c>
+      <c r="C122" s="10">
+        <v>60</v>
+      </c>
+      <c r="D122" s="10">
+        <v>12</v>
+      </c>
+      <c r="E122" s="10">
+        <v>1</v>
+      </c>
+      <c r="F122" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A123">
+        <v>-1</v>
+      </c>
+      <c r="B123" s="15">
+        <f t="shared" si="2"/>
+        <v>7260</v>
+      </c>
+      <c r="C123" s="10">
+        <v>60</v>
+      </c>
+      <c r="D123" s="10">
+        <v>12</v>
+      </c>
+      <c r="E123" s="10">
+        <v>1</v>
+      </c>
+      <c r="F123" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A124">
+        <v>-1</v>
+      </c>
+      <c r="B124" s="15">
+        <f t="shared" si="2"/>
+        <v>7320</v>
+      </c>
+      <c r="C124" s="10">
+        <v>60</v>
+      </c>
+      <c r="D124" s="10">
+        <v>12</v>
+      </c>
+      <c r="E124" s="10">
+        <v>1</v>
+      </c>
+      <c r="F124" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A125">
+        <v>-1</v>
+      </c>
+      <c r="B125" s="15">
+        <f t="shared" si="2"/>
+        <v>7380</v>
+      </c>
+      <c r="C125" s="10">
+        <v>60</v>
+      </c>
+      <c r="D125" s="10">
+        <v>12</v>
+      </c>
+      <c r="E125" s="10">
+        <v>1</v>
+      </c>
+      <c r="F125" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A126">
+        <v>-1</v>
+      </c>
+      <c r="B126" s="15">
+        <f t="shared" si="2"/>
+        <v>7440</v>
+      </c>
+      <c r="C126" s="10">
+        <v>60</v>
+      </c>
+      <c r="D126" s="10">
+        <v>12</v>
+      </c>
+      <c r="E126" s="10">
+        <v>1</v>
+      </c>
+      <c r="F126" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A127">
+        <v>-1</v>
+      </c>
+      <c r="B127" s="15">
+        <f t="shared" si="2"/>
+        <v>7500</v>
+      </c>
+      <c r="C127" s="10">
+        <v>60</v>
+      </c>
+      <c r="D127" s="10">
+        <v>12</v>
+      </c>
+      <c r="E127" s="10">
+        <v>1</v>
+      </c>
+      <c r="F127" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A128">
+        <v>-1</v>
+      </c>
+      <c r="B128" s="15">
+        <f t="shared" si="2"/>
+        <v>7560</v>
+      </c>
+      <c r="C128" s="10">
+        <v>60</v>
+      </c>
+      <c r="D128" s="10">
+        <v>12</v>
+      </c>
+      <c r="E128" s="10">
+        <v>1</v>
+      </c>
+      <c r="F128" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A129">
+        <v>-1</v>
+      </c>
+      <c r="B129" s="15">
+        <f t="shared" si="2"/>
+        <v>7620</v>
+      </c>
+      <c r="C129" s="10">
+        <v>60</v>
+      </c>
+      <c r="D129" s="10">
+        <v>12</v>
+      </c>
+      <c r="E129" s="10">
+        <v>1</v>
+      </c>
+      <c r="F129" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A130">
+        <v>-1</v>
+      </c>
+      <c r="B130" s="15">
+        <f t="shared" si="2"/>
+        <v>7680</v>
+      </c>
+      <c r="C130" s="10">
+        <v>60</v>
+      </c>
+      <c r="D130" s="10">
+        <v>12</v>
+      </c>
+      <c r="E130" s="10">
+        <v>1</v>
+      </c>
+      <c r="F130" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A131">
+        <v>-1</v>
+      </c>
+      <c r="B131" s="15">
+        <f t="shared" si="2"/>
+        <v>7740</v>
+      </c>
+      <c r="C131" s="10">
+        <v>60</v>
+      </c>
+      <c r="D131" s="10">
+        <v>12</v>
+      </c>
+      <c r="E131" s="10">
+        <v>1</v>
+      </c>
+      <c r="F131" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A132">
+        <v>-1</v>
+      </c>
+      <c r="B132" s="15">
+        <f t="shared" si="2"/>
+        <v>7800</v>
+      </c>
+      <c r="C132" s="10">
+        <v>60</v>
+      </c>
+      <c r="D132" s="10">
+        <v>12</v>
+      </c>
+      <c r="E132" s="10">
+        <v>1</v>
+      </c>
+      <c r="F132" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A133">
+        <v>-1</v>
+      </c>
+      <c r="B133" s="15">
+        <f t="shared" si="2"/>
+        <v>7860</v>
+      </c>
+      <c r="C133" s="10">
+        <v>60</v>
+      </c>
+      <c r="D133" s="10">
+        <v>12</v>
+      </c>
+      <c r="E133" s="10">
+        <v>1</v>
+      </c>
+      <c r="F133" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A134">
+        <v>-1</v>
+      </c>
+      <c r="B134" s="15">
+        <f t="shared" si="2"/>
+        <v>7920</v>
+      </c>
+      <c r="C134" s="10">
+        <v>60</v>
+      </c>
+      <c r="D134" s="10">
+        <v>12</v>
+      </c>
+      <c r="E134" s="10">
+        <v>1</v>
+      </c>
+      <c r="F134" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A135">
+        <v>-1</v>
+      </c>
+      <c r="B135" s="15">
+        <f t="shared" si="2"/>
+        <v>7980</v>
+      </c>
+      <c r="C135" s="10">
+        <v>60</v>
+      </c>
+      <c r="D135" s="10">
+        <v>12</v>
+      </c>
+      <c r="E135" s="10">
+        <v>1</v>
+      </c>
+      <c r="F135" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A136">
+        <v>-1</v>
+      </c>
+      <c r="B136" s="15">
+        <f t="shared" si="2"/>
+        <v>8040</v>
+      </c>
+      <c r="C136" s="10">
+        <v>60</v>
+      </c>
+      <c r="D136" s="10">
+        <v>12</v>
+      </c>
+      <c r="E136" s="10">
+        <v>1</v>
+      </c>
+      <c r="F136" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A137">
+        <v>-1</v>
+      </c>
+      <c r="B137" s="15">
+        <f t="shared" si="2"/>
+        <v>8100</v>
+      </c>
+      <c r="C137" s="10">
+        <v>60</v>
+      </c>
+      <c r="D137" s="10">
+        <v>12</v>
+      </c>
+      <c r="E137" s="10">
+        <v>1</v>
+      </c>
+      <c r="F137" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A138">
+        <v>-1</v>
+      </c>
+      <c r="B138" s="15">
+        <f t="shared" si="2"/>
+        <v>8160</v>
+      </c>
+      <c r="C138" s="10">
+        <v>60</v>
+      </c>
+      <c r="D138" s="10">
+        <v>12</v>
+      </c>
+      <c r="E138" s="10">
+        <v>1</v>
+      </c>
+      <c r="F138" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A139">
+        <v>-1</v>
+      </c>
+      <c r="B139" s="15">
+        <f t="shared" si="2"/>
+        <v>8220</v>
+      </c>
+      <c r="C139" s="10">
+        <v>60</v>
+      </c>
+      <c r="D139" s="10">
+        <v>12</v>
+      </c>
+      <c r="E139" s="10">
+        <v>1</v>
+      </c>
+      <c r="F139" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A140">
+        <v>-1</v>
+      </c>
+      <c r="B140" s="15">
+        <f t="shared" si="2"/>
+        <v>8280</v>
+      </c>
+      <c r="C140" s="10">
+        <v>60</v>
+      </c>
+      <c r="D140" s="10">
+        <v>12</v>
+      </c>
+      <c r="E140" s="10">
+        <v>1</v>
+      </c>
+      <c r="F140" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A141">
+        <v>-1</v>
+      </c>
+      <c r="B141" s="15">
+        <f t="shared" si="2"/>
+        <v>8340</v>
+      </c>
+      <c r="C141" s="10">
+        <v>60</v>
+      </c>
+      <c r="D141" s="10">
+        <v>12</v>
+      </c>
+      <c r="E141" s="10">
+        <v>1</v>
+      </c>
+      <c r="F141" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A142">
+        <v>-1</v>
+      </c>
+      <c r="B142" s="15">
+        <f t="shared" si="2"/>
+        <v>8400</v>
+      </c>
+      <c r="C142" s="10">
+        <v>60</v>
+      </c>
+      <c r="D142" s="10">
+        <v>12</v>
+      </c>
+      <c r="E142" s="10">
+        <v>1</v>
+      </c>
+      <c r="F142" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A143">
+        <v>-1</v>
+      </c>
+      <c r="B143" s="15">
+        <f t="shared" si="2"/>
+        <v>8460</v>
+      </c>
+      <c r="C143" s="10">
+        <v>60</v>
+      </c>
+      <c r="D143" s="10">
+        <v>12</v>
+      </c>
+      <c r="E143" s="10">
+        <v>1</v>
+      </c>
+      <c r="F143" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A144">
+        <v>-1</v>
+      </c>
+      <c r="B144" s="15">
+        <f t="shared" si="2"/>
+        <v>8520</v>
+      </c>
+      <c r="C144" s="10">
+        <v>60</v>
+      </c>
+      <c r="D144" s="10">
+        <v>12</v>
+      </c>
+      <c r="E144" s="10">
+        <v>1</v>
+      </c>
+      <c r="F144" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A145">
+        <v>-1</v>
+      </c>
+      <c r="B145" s="15">
+        <f t="shared" si="2"/>
+        <v>8580</v>
+      </c>
+      <c r="C145" s="10">
+        <v>60</v>
+      </c>
+      <c r="D145" s="10">
+        <v>12</v>
+      </c>
+      <c r="E145" s="10">
+        <v>1</v>
+      </c>
+      <c r="F145" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A146">
+        <v>-1</v>
+      </c>
+      <c r="B146" s="15">
+        <f t="shared" si="2"/>
+        <v>8640</v>
+      </c>
+      <c r="C146" s="10">
+        <v>60</v>
+      </c>
+      <c r="D146" s="10">
+        <v>12</v>
+      </c>
+      <c r="E146" s="10">
+        <v>1</v>
+      </c>
+      <c r="F146" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A147">
+        <v>-1</v>
+      </c>
+      <c r="B147" s="15">
+        <f t="shared" si="2"/>
+        <v>8700</v>
+      </c>
+      <c r="C147" s="10">
+        <v>60</v>
+      </c>
+      <c r="D147" s="10">
+        <v>12</v>
+      </c>
+      <c r="E147" s="10">
+        <v>1</v>
+      </c>
+      <c r="F147" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A148">
+        <v>-1</v>
+      </c>
+      <c r="B148" s="15">
+        <f t="shared" si="2"/>
+        <v>8760</v>
+      </c>
+      <c r="C148" s="10">
+        <v>60</v>
+      </c>
+      <c r="D148" s="10">
+        <v>12</v>
+      </c>
+      <c r="E148" s="10">
+        <v>1</v>
+      </c>
+      <c r="F148" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A149">
+        <v>-1</v>
+      </c>
+      <c r="B149" s="15">
+        <f t="shared" si="2"/>
+        <v>8820</v>
+      </c>
+      <c r="C149" s="10">
+        <v>60</v>
+      </c>
+      <c r="D149" s="10">
+        <v>12</v>
+      </c>
+      <c r="E149" s="10">
+        <v>1</v>
+      </c>
+      <c r="F149" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A150">
+        <v>-1</v>
+      </c>
+      <c r="B150" s="15">
+        <f t="shared" si="2"/>
+        <v>8880</v>
+      </c>
+      <c r="C150" s="10">
+        <v>60</v>
+      </c>
+      <c r="D150" s="10">
+        <v>12</v>
+      </c>
+      <c r="E150" s="10">
+        <v>1</v>
+      </c>
+      <c r="F150" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A151">
+        <v>-1</v>
+      </c>
+      <c r="B151" s="15">
+        <f t="shared" si="2"/>
+        <v>8940</v>
+      </c>
+      <c r="C151" s="10">
+        <v>60</v>
+      </c>
+      <c r="D151" s="10">
+        <v>12</v>
+      </c>
+      <c r="E151" s="10">
+        <v>1</v>
+      </c>
+      <c r="F151" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A152">
+        <v>-1</v>
+      </c>
+      <c r="B152" s="15">
+        <f t="shared" si="2"/>
+        <v>9000</v>
+      </c>
+      <c r="C152" s="10">
+        <v>60</v>
+      </c>
+      <c r="D152" s="10">
+        <v>12</v>
+      </c>
+      <c r="E152" s="10">
+        <v>1</v>
+      </c>
+      <c r="F152" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A153">
+        <v>-1</v>
+      </c>
+      <c r="B153" s="15">
+        <f t="shared" si="2"/>
+        <v>9060</v>
+      </c>
+      <c r="C153" s="10">
+        <v>60</v>
+      </c>
+      <c r="D153" s="10">
+        <v>12</v>
+      </c>
+      <c r="E153" s="10">
+        <v>1</v>
+      </c>
+      <c r="F153" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A154">
+        <v>-1</v>
+      </c>
+      <c r="B154" s="15">
+        <f t="shared" si="2"/>
+        <v>9120</v>
+      </c>
+      <c r="C154" s="10">
+        <v>60</v>
+      </c>
+      <c r="D154" s="10">
+        <v>12</v>
+      </c>
+      <c r="E154" s="10">
+        <v>1</v>
+      </c>
+      <c r="F154" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A155">
+        <v>-1</v>
+      </c>
+      <c r="B155" s="15">
+        <f t="shared" si="2"/>
+        <v>9180</v>
+      </c>
+      <c r="C155" s="10">
+        <v>60</v>
+      </c>
+      <c r="D155" s="10">
+        <v>12</v>
+      </c>
+      <c r="E155" s="10">
+        <v>1</v>
+      </c>
+      <c r="F155" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A156">
+        <v>-1</v>
+      </c>
+      <c r="B156" s="15">
+        <f t="shared" si="2"/>
+        <v>9240</v>
+      </c>
+      <c r="C156" s="10">
+        <v>60</v>
+      </c>
+      <c r="D156" s="10">
+        <v>12</v>
+      </c>
+      <c r="E156" s="10">
+        <v>1</v>
+      </c>
+      <c r="F156" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A157">
+        <v>-1</v>
+      </c>
+      <c r="B157" s="15">
+        <f t="shared" si="2"/>
+        <v>9300</v>
+      </c>
+      <c r="C157" s="10">
+        <v>60</v>
+      </c>
+      <c r="D157" s="10">
+        <v>12</v>
+      </c>
+      <c r="E157" s="10">
+        <v>1</v>
+      </c>
+      <c r="F157" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A158">
+        <v>-1</v>
+      </c>
+      <c r="B158" s="15">
+        <f t="shared" si="2"/>
+        <v>9360</v>
+      </c>
+      <c r="C158" s="10">
+        <v>60</v>
+      </c>
+      <c r="D158" s="10">
+        <v>12</v>
+      </c>
+      <c r="E158" s="10">
+        <v>1</v>
+      </c>
+      <c r="F158" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A159">
+        <v>-1</v>
+      </c>
+      <c r="B159" s="15">
+        <f t="shared" si="2"/>
+        <v>9420</v>
+      </c>
+      <c r="C159" s="10">
+        <v>60</v>
+      </c>
+      <c r="D159" s="10">
+        <v>12</v>
+      </c>
+      <c r="E159" s="10">
+        <v>1</v>
+      </c>
+      <c r="F159" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A160">
+        <v>-1</v>
+      </c>
+      <c r="B160" s="15">
+        <f t="shared" si="2"/>
+        <v>9480</v>
+      </c>
+      <c r="C160" s="10">
+        <v>60</v>
+      </c>
+      <c r="D160" s="10">
+        <v>12</v>
+      </c>
+      <c r="E160" s="10">
+        <v>1</v>
+      </c>
+      <c r="F160" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A161">
+        <v>-1</v>
+      </c>
+      <c r="B161" s="15">
+        <f t="shared" si="2"/>
+        <v>9540</v>
+      </c>
+      <c r="C161" s="10">
+        <v>60</v>
+      </c>
+      <c r="D161" s="10">
+        <v>12</v>
+      </c>
+      <c r="E161" s="10">
+        <v>1</v>
+      </c>
+      <c r="F161" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A162">
+        <v>-1</v>
+      </c>
+      <c r="B162" s="15">
+        <f t="shared" ref="B162:B180" si="3">B161+C162</f>
+        <v>9600</v>
+      </c>
+      <c r="C162" s="10">
+        <v>60</v>
+      </c>
+      <c r="D162" s="10">
+        <v>12</v>
+      </c>
+      <c r="E162" s="10">
+        <v>1</v>
+      </c>
+      <c r="F162" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A163">
+        <v>-1</v>
+      </c>
+      <c r="B163" s="15">
+        <f t="shared" si="3"/>
+        <v>9660</v>
+      </c>
+      <c r="C163" s="10">
+        <v>60</v>
+      </c>
+      <c r="D163" s="10">
+        <v>12</v>
+      </c>
+      <c r="E163" s="10">
+        <v>1</v>
+      </c>
+      <c r="F163" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A164">
+        <v>-1</v>
+      </c>
+      <c r="B164" s="15">
+        <f t="shared" si="3"/>
+        <v>9720</v>
+      </c>
+      <c r="C164" s="10">
+        <v>60</v>
+      </c>
+      <c r="D164" s="10">
+        <v>12</v>
+      </c>
+      <c r="E164" s="10">
+        <v>1</v>
+      </c>
+      <c r="F164" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A165">
+        <v>-1</v>
+      </c>
+      <c r="B165" s="15">
+        <f t="shared" si="3"/>
+        <v>9780</v>
+      </c>
+      <c r="C165" s="10">
+        <v>60</v>
+      </c>
+      <c r="D165" s="10">
+        <v>12</v>
+      </c>
+      <c r="E165" s="10">
+        <v>1</v>
+      </c>
+      <c r="F165" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A166">
+        <v>-1</v>
+      </c>
+      <c r="B166" s="15">
+        <f t="shared" si="3"/>
+        <v>9840</v>
+      </c>
+      <c r="C166" s="10">
+        <v>60</v>
+      </c>
+      <c r="D166" s="10">
+        <v>12</v>
+      </c>
+      <c r="E166" s="10">
+        <v>1</v>
+      </c>
+      <c r="F166" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A167">
+        <v>-1</v>
+      </c>
+      <c r="B167" s="15">
+        <f t="shared" si="3"/>
+        <v>9900</v>
+      </c>
+      <c r="C167" s="10">
+        <v>60</v>
+      </c>
+      <c r="D167" s="10">
+        <v>12</v>
+      </c>
+      <c r="E167" s="10">
+        <v>1</v>
+      </c>
+      <c r="F167" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A168">
+        <v>-1</v>
+      </c>
+      <c r="B168" s="15">
+        <f t="shared" si="3"/>
+        <v>9960</v>
+      </c>
+      <c r="C168" s="10">
+        <v>60</v>
+      </c>
+      <c r="D168" s="10">
+        <v>12</v>
+      </c>
+      <c r="E168" s="10">
+        <v>1</v>
+      </c>
+      <c r="F168" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A169">
+        <v>-1</v>
+      </c>
+      <c r="B169" s="15">
+        <f t="shared" si="3"/>
+        <v>10020</v>
+      </c>
+      <c r="C169" s="10">
+        <v>60</v>
+      </c>
+      <c r="D169" s="10">
+        <v>12</v>
+      </c>
+      <c r="E169" s="10">
+        <v>1</v>
+      </c>
+      <c r="F169" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A170">
+        <v>-1</v>
+      </c>
+      <c r="B170" s="15">
+        <f t="shared" si="3"/>
+        <v>10080</v>
+      </c>
+      <c r="C170" s="10">
+        <v>60</v>
+      </c>
+      <c r="D170" s="10">
+        <v>12</v>
+      </c>
+      <c r="E170" s="10">
+        <v>1</v>
+      </c>
+      <c r="F170" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A171">
+        <v>-1</v>
+      </c>
+      <c r="B171" s="15">
+        <f t="shared" si="3"/>
+        <v>10140</v>
+      </c>
+      <c r="C171" s="10">
+        <v>60</v>
+      </c>
+      <c r="D171" s="10">
+        <v>12</v>
+      </c>
+      <c r="E171" s="10">
+        <v>1</v>
+      </c>
+      <c r="F171" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A172">
+        <v>-1</v>
+      </c>
+      <c r="B172" s="15">
+        <f t="shared" si="3"/>
+        <v>10200</v>
+      </c>
+      <c r="C172" s="10">
+        <v>60</v>
+      </c>
+      <c r="D172" s="10">
+        <v>12</v>
+      </c>
+      <c r="E172" s="10">
+        <v>1</v>
+      </c>
+      <c r="F172" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A173">
+        <v>-1</v>
+      </c>
+      <c r="B173" s="15">
+        <f t="shared" si="3"/>
+        <v>10260</v>
+      </c>
+      <c r="C173" s="10">
+        <v>60</v>
+      </c>
+      <c r="D173" s="10">
+        <v>12</v>
+      </c>
+      <c r="E173" s="10">
+        <v>1</v>
+      </c>
+      <c r="F173" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A174">
+        <v>-1</v>
+      </c>
+      <c r="B174" s="15">
+        <f t="shared" si="3"/>
+        <v>10320</v>
+      </c>
+      <c r="C174" s="10">
+        <v>60</v>
+      </c>
+      <c r="D174" s="10">
+        <v>12</v>
+      </c>
+      <c r="E174" s="10">
+        <v>1</v>
+      </c>
+      <c r="F174" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A175">
+        <v>-1</v>
+      </c>
+      <c r="B175" s="15">
+        <f t="shared" si="3"/>
+        <v>10380</v>
+      </c>
+      <c r="C175" s="10">
+        <v>60</v>
+      </c>
+      <c r="D175" s="10">
+        <v>12</v>
+      </c>
+      <c r="E175" s="10">
+        <v>1</v>
+      </c>
+      <c r="F175" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A176">
+        <v>-1</v>
+      </c>
+      <c r="B176" s="15">
+        <f t="shared" si="3"/>
+        <v>10440</v>
+      </c>
+      <c r="C176" s="10">
+        <v>60</v>
+      </c>
+      <c r="D176" s="10">
+        <v>12</v>
+      </c>
+      <c r="E176" s="10">
+        <v>1</v>
+      </c>
+      <c r="F176" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A177">
+        <v>-1</v>
+      </c>
+      <c r="B177" s="15">
+        <f t="shared" si="3"/>
+        <v>10500</v>
+      </c>
+      <c r="C177" s="10">
+        <v>60</v>
+      </c>
+      <c r="D177" s="10">
+        <v>12</v>
+      </c>
+      <c r="E177" s="10">
+        <v>1</v>
+      </c>
+      <c r="F177" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A178">
+        <v>-1</v>
+      </c>
+      <c r="B178" s="15">
+        <f t="shared" si="3"/>
+        <v>10560</v>
+      </c>
+      <c r="C178" s="10">
+        <v>60</v>
+      </c>
+      <c r="D178" s="10">
+        <v>12</v>
+      </c>
+      <c r="E178" s="10">
+        <v>1</v>
+      </c>
+      <c r="F178" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A179">
+        <v>-1</v>
+      </c>
+      <c r="B179" s="15">
+        <f t="shared" si="3"/>
+        <v>10620</v>
+      </c>
+      <c r="C179" s="10">
+        <v>60</v>
+      </c>
+      <c r="D179" s="10">
+        <v>12</v>
+      </c>
+      <c r="E179" s="10">
+        <v>1</v>
+      </c>
+      <c r="F179" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A180">
+        <v>-1</v>
+      </c>
+      <c r="B180" s="15">
+        <f t="shared" si="3"/>
+        <v>10680</v>
+      </c>
+      <c r="C180" s="10">
+        <v>60</v>
+      </c>
+      <c r="D180" s="10">
+        <v>12</v>
+      </c>
+      <c r="E180" s="10">
+        <v>1</v>
+      </c>
+      <c r="F180" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A181">
+        <v>-1</v>
+      </c>
+      <c r="B181" s="15">
+        <f t="shared" ref="B181:B183" si="4">B180+C181</f>
+        <v>10740</v>
+      </c>
+      <c r="C181" s="10">
+        <v>60</v>
+      </c>
+      <c r="D181" s="10">
+        <v>12</v>
+      </c>
+      <c r="E181" s="10">
+        <v>1</v>
+      </c>
+      <c r="F181" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A182">
+        <v>-1</v>
+      </c>
+      <c r="B182" s="15">
+        <f t="shared" si="4"/>
+        <v>10800</v>
+      </c>
+      <c r="C182" s="10">
+        <v>60</v>
+      </c>
+      <c r="D182" s="10">
+        <v>12</v>
+      </c>
+      <c r="E182" s="10">
+        <v>1</v>
+      </c>
+      <c r="F182" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B183" s="15"/>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
+      <c r="F183" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12518,22 +15766,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A3" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>76</v>
@@ -12542,164 +15790,104 @@
         <v>78</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G2" s="17">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F3" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="17">
-        <v>5</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>393</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G4" s="17">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
         <v>3</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>4</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G5" s="17">
-        <v>10</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1E-3</v>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0.1</v>
@@ -12707,18 +15895,309 @@
       <c r="F6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G6" s="17">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="H6" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>396</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>389</v>
-      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="F22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Henry problem nicely finihed wih two vafiants and video's. Answer verified to example 51 in publicaion by the Modflow 6 Development Team (203).
</commit_message>
<xml_diff>
--- a/Projects/Density/cases/Henry/Henry.xlsx
+++ b/Projects/Density/cases/Henry/Henry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Density/cases/Henry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185CF7E7-D377-B746-8CD1-D6355F384A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB15FEB-AEEB-D046-959E-7BF59997216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="-26960" windowWidth="30600" windowHeight="19860" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2470,11 +2470,11 @@
         <v>314</v>
       </c>
       <c r="B34" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;====</v>
+        <v/>
       </c>
       <c r="D34" s="13" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
All cross sectioins now ok.
</commit_message>
<xml_diff>
--- a/Projects/Density/cases/Henry/Henry.xlsx
+++ b/Projects/Density/cases/Henry/Henry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Density/cases/Henry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB15FEB-AEEB-D046-959E-7BF59997216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FFD3CA-B40A-2649-BD61-84AB35803538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="-26960" windowWidth="30600" windowHeight="19860" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11860" yWindow="-26960" windowWidth="30600" windowHeight="19860" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -2470,11 +2470,11 @@
         <v>314</v>
       </c>
       <c r="B34" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
Iconvert set to one everywhere to ensure conveting between Sy and Ss in transient flow. Inactive flow through cells are interpolated from the first actie cell above and below. Solves curious concentrations. gr.Zpm now ues gr.Z[0] as top and gr.Z[-1] as bottom, wich yield nicer concentration contour plots.
</commit_message>
<xml_diff>
--- a/Projects/Density/cases/Henry/Henry.xlsx
+++ b/Projects/Density/cases/Henry/Henry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Density/cases/Henry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FFD3CA-B40A-2649-BD61-84AB35803538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391A376A-534C-0044-90F0-937325A67DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11860" yWindow="-26960" windowWidth="30600" windowHeight="19860" tabRatio="751" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11860" yWindow="-26960" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -1959,7 +1959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -3535,8 +3535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A404" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C426" sqref="C426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7957,7 +7957,7 @@
         <v>26</v>
       </c>
       <c r="C425">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="426" spans="1:8" x14ac:dyDescent="0.15">

</xml_diff>